<commit_message>
Improvements: - Improved: Reduce the Save Information after the Lipid Identification
BugFix:
- Fixed: Specific ions file accure masses
- Temporaty Fixed: for one m/z value to have 2 fragments identification
</commit_message>
<xml_diff>
--- a/ConfigurationFiles/02-Specific_ions.xlsx
+++ b/ConfigurationFiles/02-Specific_ions.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{CDBD874B-2ED7-46D8-B163-4CC3CA2969C2}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -309,7 +310,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
@@ -671,11 +672,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1007,7 +1008,7 @@
         <v>3</v>
       </c>
       <c r="C14" s="1">
-        <v>184.06</v>
+        <v>184.07390000000001</v>
       </c>
       <c r="D14" t="s">
         <v>84</v>
@@ -1146,7 +1147,7 @@
         <v>3</v>
       </c>
       <c r="C20" s="3">
-        <v>142</v>
+        <v>142.02690000000001</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>83</v>
@@ -1353,8 +1354,8 @@
       <c r="B31" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C31" s="1">
-        <v>186</v>
+      <c r="C31" s="3">
+        <v>186.01679999999999</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>85</v>

</xml_diff>